<commit_message>
Update all of the accounting spreadsheets with the latest financial information
Updates expenses.xlsx, production_units.xlsx, revenues.xlsx and reports.xlsx with new data, also creates a new expenses report.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: cdd29b5b-2652-4b10-9df1-39d8388fd989
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7193f0d6-a227-4876-829b-be28091fbb85/1ec00f7d-0d0d-4a85-854b-fcca27f35d44.jpg
</commit_message>
<xml_diff>
--- a/data/expenses.xlsx
+++ b/data/expenses.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>id</t>
   </si>
@@ -29,6 +29,114 @@
   </si>
   <si>
     <t>category</t>
+  </si>
+  <si>
+    <t>baseAmount</t>
+  </si>
+  <si>
+    <t>gstRate</t>
+  </si>
+  <si>
+    <t>gstAmount</t>
+  </si>
+  <si>
+    <t>hsn</t>
+  </si>
+  <si>
+    <t>invoiceNumber</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Office Supplies Purchase</t>
+  </si>
+  <si>
+    <t>5900</t>
+  </si>
+  <si>
+    <t>2025-05-05T08:48:51.663Z</t>
+  </si>
+  <si>
+    <t>Office Supplies</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>900</t>
+  </si>
+  <si>
+    <t>4901</t>
+  </si>
+  <si>
+    <t>INV-001</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>Raw Material Purchase</t>
+  </si>
+  <si>
+    <t>10500</t>
+  </si>
+  <si>
+    <t>Raw Materials</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>INV-002</t>
+  </si>
+  <si>
+    <t>Equipment Maintenance</t>
+  </si>
+  <si>
+    <t>11800</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>1800</t>
+  </si>
+  <si>
+    <t>8471</t>
+  </si>
+  <si>
+    <t>INV-003</t>
+  </si>
+  <si>
+    <t>Transportation Services</t>
+  </si>
+  <si>
+    <t>5250</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>9965</t>
+  </si>
+  <si>
+    <t>INV-004</t>
   </si>
 </sst>
 </file>
@@ -419,17 +527,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:L5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -447,6 +562,176 @@
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>